<commit_message>
Add validation data processing and evaluation functions
- Implemented `preprocess_validation_data` to standardize and prepare validation datasets from different countries.
- Added `evaluate_model` function to assess model performance on validation data, including metrics calculation.
- Created utility functions for plotting ROC curves and confusion matrices.
- Introduced SHAP force plot functionality for model interpretability.
- Generated validation metrics for various models and saved results to CSV files.
- Added comprehensive data cleaning and feature engineering steps in `validation.py`.
</commit_message>
<xml_diff>
--- a/data/fatigue_ml_data_validation_scotland.xlsx
+++ b/data/fatigue_ml_data_validation_scotland.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chershiongchuah/Developer/machine_learning_for_ibd_fatigue/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEE5269-C246-2847-A3D1-C55862185930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="510" windowWidth="7965" windowHeight="7575"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="25360" windowHeight="26340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fatigue_validation" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="136">
   <si>
     <t>age</t>
   </si>
@@ -366,9 +372,6 @@
     <t>Clinical Setting (inpatient, outpatient, endoscopy, infusion unit, etc.)</t>
   </si>
   <si>
-    <t>Date Referred</t>
-  </si>
-  <si>
     <t>Outpatient</t>
   </si>
   <si>
@@ -418,13 +421,22 @@
   </si>
   <si>
     <t xml:space="preserve">Solomon </t>
+  </si>
+  <si>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Endoscopy GI DAMPs</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -946,7 +958,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -961,7 +973,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1329,73 +1340,73 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.83203125" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5" style="7" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" style="7" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21" style="5" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="37.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="37.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5" style="5" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.5" style="5" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5" style="5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="24.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="48" max="49" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="3" customFormat="1" ht="20.25">
+    <row r="1" spans="1:49" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>111</v>
       </c>
@@ -1403,7 +1414,7 @@
         <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>77</v>
@@ -1544,12 +1555,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
-      <c r="A2" s="14" t="s">
-        <v>127</v>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="12">
         <v>45722</v>
@@ -1570,7 +1581,7 @@
         <v>86.8</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
         <v>59</v>
@@ -1645,12 +1656,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
-      <c r="A3" s="14" t="s">
-        <v>127</v>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="12">
         <v>45722</v>
@@ -1671,7 +1682,7 @@
         <v>90.8</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
         <v>58</v>
@@ -1722,7 +1733,7 @@
         <v>291</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC3" s="7">
         <v>83</v>
@@ -1734,7 +1745,7 @@
         <v>3.9</v>
       </c>
       <c r="AF3" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AG3" s="7">
         <v>42</v>
@@ -1749,12 +1760,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
-      <c r="A4" s="14" t="s">
-        <v>127</v>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="12">
         <v>45722</v>
@@ -1775,7 +1786,7 @@
         <v>99.6</v>
       </c>
       <c r="I4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
@@ -1850,12 +1861,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
-      <c r="A5" s="14" t="s">
-        <v>127</v>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="12">
         <v>45722</v>
@@ -1876,7 +1887,7 @@
         <v>59.3</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J5" t="s">
         <v>57</v>
@@ -1945,12 +1956,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
-      <c r="A6" s="14" t="s">
-        <v>127</v>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="12">
         <v>45722</v>
@@ -1971,7 +1982,7 @@
         <v>81.2</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
         <v>58</v>
@@ -2049,12 +2060,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
-      <c r="A7" s="14" t="s">
-        <v>127</v>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="12">
         <v>45722</v>
@@ -2075,7 +2086,7 @@
         <v>67.3</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J7" t="s">
         <v>58</v>
@@ -2150,12 +2161,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
-      <c r="A8" s="14" t="s">
-        <v>127</v>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="12">
         <v>45722</v>
@@ -2176,7 +2187,7 @@
         <v>78.7</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J8" t="s">
         <v>58</v>
@@ -2251,12 +2262,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
-      <c r="A9" s="14" t="s">
-        <v>127</v>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="12">
         <v>45720</v>
@@ -2277,7 +2288,7 @@
         <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J9" t="s">
         <v>58</v>
@@ -2346,15 +2357,15 @@
         <v>40</v>
       </c>
       <c r="AH9" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:49">
-      <c r="A10" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="12">
         <v>45720</v>
@@ -2375,7 +2386,7 @@
         <v>111.6</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J10" t="s">
         <v>58</v>
@@ -2450,12 +2461,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
-      <c r="A11" s="14" t="s">
-        <v>127</v>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="12">
         <v>45720</v>
@@ -2476,7 +2487,7 @@
         <v>105.9</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J11" t="s">
         <v>58</v>
@@ -2551,12 +2562,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
-      <c r="A12" s="14" t="s">
-        <v>127</v>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="12">
         <v>45713</v>
@@ -2571,13 +2582,13 @@
         <v>109</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J12" t="s">
         <v>58</v>
@@ -2601,60 +2612,60 @@
         <v>67</v>
       </c>
       <c r="S12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH12" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>126</v>
       </c>
-      <c r="T12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="W12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="X12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH12" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:49">
-      <c r="A13" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="12">
         <v>45713</v>
@@ -2669,13 +2680,13 @@
         <v>109</v>
       </c>
       <c r="G13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H13">
         <v>105</v>
       </c>
       <c r="I13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" t="s">
         <v>58</v>
@@ -2744,18 +2755,18 @@
         <v>38</v>
       </c>
       <c r="AH13" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AO13" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>126</v>
       </c>
-      <c r="AO13" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:49">
-      <c r="A14" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="12">
         <v>45713</v>
@@ -2776,7 +2787,7 @@
         <v>81.8</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J14" t="s">
         <v>58</v>
@@ -2851,12 +2862,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
-      <c r="A15" s="14" t="s">
-        <v>127</v>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" s="12">
         <v>45713</v>
@@ -2877,7 +2888,7 @@
         <v>84.1</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J15" t="s">
         <v>58</v>
@@ -2949,12 +2960,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
-      <c r="A16" s="14" t="s">
-        <v>127</v>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="12">
         <v>45713</v>
@@ -2975,7 +2986,7 @@
         <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J16" t="s">
         <v>57</v>
@@ -2993,60 +3004,60 @@
         <v>67</v>
       </c>
       <c r="S16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH16" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>126</v>
       </c>
-      <c r="T16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="X16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH16" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:49">
-      <c r="A17" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="12">
         <v>45701</v>
@@ -3067,7 +3078,7 @@
         <v>58.2</v>
       </c>
       <c r="I17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J17" t="s">
         <v>58</v>
@@ -3136,15 +3147,15 @@
         <v>36</v>
       </c>
       <c r="AH17" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:49">
-      <c r="A18" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="12">
         <v>45701</v>
@@ -3165,7 +3176,7 @@
         <v>59</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J18" t="s">
         <v>58</v>
@@ -3243,12 +3254,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
-      <c r="A19" s="14" t="s">
-        <v>127</v>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="12">
         <v>45701</v>
@@ -3269,7 +3280,7 @@
         <v>86</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J19" t="s">
         <v>57</v>
@@ -3341,12 +3352,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
-      <c r="A20" s="14" t="s">
-        <v>127</v>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="12">
         <v>45729</v>
@@ -3367,7 +3378,7 @@
         <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J20" t="s">
         <v>58</v>
@@ -3436,18 +3447,18 @@
         <v>29</v>
       </c>
       <c r="AH20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ20" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>126</v>
       </c>
-      <c r="AQ20" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:49">
-      <c r="A21" s="14" t="s">
-        <v>127</v>
-      </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="12">
         <v>45729</v>
@@ -3468,7 +3479,7 @@
         <v>85</v>
       </c>
       <c r="I21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J21" t="s">
         <v>58</v>
@@ -3537,18 +3548,18 @@
         <v>42</v>
       </c>
       <c r="AH21" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AQ21" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" s="12">
         <v>45729</v>
@@ -3569,7 +3580,7 @@
         <v>77.7</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J22" t="s">
         <v>57</v>
@@ -3593,12 +3604,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="12">
         <v>45729</v>
@@ -3619,7 +3630,7 @@
         <v>85.2</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J23" t="s">
         <v>58</v>
@@ -3649,12 +3660,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" s="12">
         <v>45744</v>
@@ -3675,7 +3686,7 @@
         <v>83.7</v>
       </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J24" t="s">
         <v>58</v>
@@ -3750,12 +3761,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" s="12">
         <v>45747</v>
@@ -3776,7 +3787,7 @@
         <v>51.9</v>
       </c>
       <c r="I25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J25" t="s">
         <v>58</v>
@@ -3851,12 +3862,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" s="12">
         <v>45743</v>
@@ -3877,7 +3888,7 @@
         <v>60.8</v>
       </c>
       <c r="I26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J26" t="s">
         <v>58</v>
@@ -3952,12 +3963,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="12">
         <v>45734</v>
@@ -3978,7 +3989,7 @@
         <v>111.5</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J27" t="s">
         <v>58</v>
@@ -4053,12 +4064,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" s="12">
         <v>45741</v>
@@ -4079,7 +4090,7 @@
         <v>100</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J28" t="s">
         <v>58</v>
@@ -4151,12 +4162,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="12">
         <v>45748</v>
@@ -4177,7 +4188,7 @@
         <v>72.5</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J29" t="s">
         <v>58</v>
@@ -4252,12 +4263,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="12">
         <v>45748</v>
@@ -4278,7 +4289,7 @@
         <v>57.2</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J30" t="s">
         <v>58</v>
@@ -4353,12 +4364,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="12">
         <v>45748</v>
@@ -4379,7 +4390,7 @@
         <v>79.2</v>
       </c>
       <c r="I31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J31" t="s">
         <v>57</v>
@@ -4442,18 +4453,18 @@
         <v>40</v>
       </c>
       <c r="AH31" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AK31" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="12">
         <v>45757</v>
@@ -4474,7 +4485,7 @@
         <v>81.900000000000006</v>
       </c>
       <c r="I32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J32" t="s">
         <v>57</v>
@@ -4546,12 +4557,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:49">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" s="12">
         <v>45757</v>
@@ -4572,7 +4583,7 @@
         <v>97</v>
       </c>
       <c r="I33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J33" t="s">
         <v>58</v>
@@ -4647,12 +4658,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:49">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="12">
         <v>45757</v>
@@ -4673,7 +4684,7 @@
         <v>78</v>
       </c>
       <c r="I34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J34" t="s">
         <v>57</v>
@@ -4745,12 +4756,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:49">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35" s="12">
         <v>45762</v>
@@ -4771,7 +4782,7 @@
         <v>83.3</v>
       </c>
       <c r="I35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J35" t="s">
         <v>58</v>
@@ -4837,12 +4848,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:49">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" s="12">
         <v>45762</v>
@@ -4863,7 +4874,7 @@
         <v>77.099999999999994</v>
       </c>
       <c r="I36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J36" t="s">
         <v>58</v>
@@ -4935,12 +4946,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:49">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C37" s="12">
         <v>45762</v>
@@ -4961,7 +4972,7 @@
         <v>113.8</v>
       </c>
       <c r="I37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J37" t="s">
         <v>58</v>
@@ -5030,12 +5041,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:49">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="12">
         <v>45764</v>
@@ -5056,7 +5067,7 @@
         <v>78.7</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J38" t="s">
         <v>58</v>
@@ -5128,12 +5139,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:49">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" s="12">
         <v>45764</v>
@@ -5154,7 +5165,7 @@
         <v>69.099999999999994</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J39" t="s">
         <v>57</v>
@@ -5172,12 +5183,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:49">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" s="12">
         <v>45769</v>
@@ -5198,7 +5209,7 @@
         <v>98</v>
       </c>
       <c r="I40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J40" t="s">
         <v>57</v>
@@ -5267,12 +5278,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:49">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="12">
         <v>45769</v>
@@ -5293,7 +5304,7 @@
         <v>67.599999999999994</v>
       </c>
       <c r="I41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J41" t="s">
         <v>58</v>
@@ -5368,12 +5379,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:49">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="12">
         <v>45769</v>
@@ -5394,7 +5405,7 @@
         <v>91.4</v>
       </c>
       <c r="I42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J42" t="s">
         <v>57</v>
@@ -5463,12 +5474,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:49">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="12">
         <v>45769</v>
@@ -5489,7 +5500,7 @@
         <v>64</v>
       </c>
       <c r="I43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J43" t="s">
         <v>57</v>
@@ -5558,12 +5569,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:49">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="12">
         <v>45769</v>
@@ -5584,7 +5595,7 @@
         <v>57.5</v>
       </c>
       <c r="I44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J44" t="s">
         <v>57</v>
@@ -5653,12 +5664,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:49">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="12">
         <v>45769</v>
@@ -5679,7 +5690,7 @@
         <v>83</v>
       </c>
       <c r="I45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J45" t="s">
         <v>57</v>
@@ -5748,12 +5759,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:49">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="12">
         <v>45769</v>
@@ -5774,7 +5785,7 @@
         <v>98.3</v>
       </c>
       <c r="I46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J46" t="s">
         <v>58</v>
@@ -5843,12 +5854,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:49">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" s="12">
         <v>45769</v>
@@ -5869,7 +5880,7 @@
         <v>83</v>
       </c>
       <c r="I47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J47" t="s">
         <v>57</v>
@@ -5878,7 +5889,7 @@
         <v>36892</v>
       </c>
       <c r="P47" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q47" s="9" t="s">
         <v>71</v>
@@ -5938,12 +5949,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:49">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="12">
         <v>45769</v>
@@ -5952,15 +5963,15 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:48">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" s="12">
         <v>45726</v>
@@ -5981,7 +5992,7 @@
         <v>75.7</v>
       </c>
       <c r="I49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J49" t="s">
         <v>58</v>
@@ -6056,12 +6067,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:48">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50" s="12">
         <v>45742</v>
@@ -6082,7 +6093,7 @@
         <v>129.19999999999999</v>
       </c>
       <c r="I50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J50" t="s">
         <v>57</v>
@@ -6091,7 +6102,7 @@
         <v>40544</v>
       </c>
       <c r="P50" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q50" s="9" t="s">
         <v>72</v>
@@ -6151,12 +6162,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:48">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="12">
         <v>45771</v>
@@ -6177,7 +6188,7 @@
         <v>43.8</v>
       </c>
       <c r="I51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>58</v>
@@ -6252,12 +6263,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:48">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="12">
         <v>45771</v>
@@ -6278,7 +6289,7 @@
         <v>152</v>
       </c>
       <c r="I52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J52" t="s">
         <v>58</v>
@@ -6347,12 +6358,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:48">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="12">
         <v>45770</v>
@@ -6373,7 +6384,7 @@
         <v>96.6</v>
       </c>
       <c r="I53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J53" t="s">
         <v>58</v>
@@ -6448,12 +6459,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:48">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="12">
         <v>45770</v>
@@ -6474,7 +6485,7 @@
         <v>57.3</v>
       </c>
       <c r="I54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J54" t="s">
         <v>58</v>
@@ -6546,16 +6557,774 @@
         <v>66</v>
       </c>
     </row>
+    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="12">
+        <v>45783</v>
+      </c>
+      <c r="D55">
+        <v>14</v>
+      </c>
+      <c r="E55">
+        <v>41</v>
+      </c>
+      <c r="F55" t="s">
+        <v>108</v>
+      </c>
+      <c r="G55">
+        <v>183</v>
+      </c>
+      <c r="H55">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="I55" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K55" s="12">
+        <v>42887</v>
+      </c>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>73</v>
+      </c>
+      <c r="R55" t="s">
+        <v>67</v>
+      </c>
+      <c r="S55">
+        <v>151</v>
+      </c>
+      <c r="T55">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U55">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="V55">
+        <v>1.7</v>
+      </c>
+      <c r="W55">
+        <v>2.52</v>
+      </c>
+      <c r="X55">
+        <v>0.41</v>
+      </c>
+      <c r="Y55">
+        <v>0.24</v>
+      </c>
+      <c r="Z55">
+        <v>0.04</v>
+      </c>
+      <c r="AA55">
+        <v>203</v>
+      </c>
+      <c r="AB55">
+        <v>4.2</v>
+      </c>
+      <c r="AC55">
+        <v>73</v>
+      </c>
+      <c r="AD55">
+        <v>140</v>
+      </c>
+      <c r="AE55">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AF55">
+        <v>1</v>
+      </c>
+      <c r="AG55">
+        <v>43</v>
+      </c>
+      <c r="AH55"/>
+      <c r="AK55" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="12">
+        <v>45784</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>23</v>
+      </c>
+      <c r="F56" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56">
+        <v>165</v>
+      </c>
+      <c r="H56">
+        <v>103.6</v>
+      </c>
+      <c r="I56" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" t="s">
+        <v>58</v>
+      </c>
+      <c r="K56" s="12">
+        <v>45329</v>
+      </c>
+      <c r="L56" t="s">
+        <v>60</v>
+      </c>
+      <c r="M56" t="s">
+        <v>63</v>
+      </c>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56" t="s">
+        <v>67</v>
+      </c>
+      <c r="S56">
+        <v>142</v>
+      </c>
+      <c r="T56">
+        <v>4.45</v>
+      </c>
+      <c r="U56">
+        <v>10.5</v>
+      </c>
+      <c r="V56">
+        <v>7.7</v>
+      </c>
+      <c r="W56">
+        <v>1.4</v>
+      </c>
+      <c r="X56">
+        <v>1</v>
+      </c>
+      <c r="Y56">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Z56">
+        <v>0.1</v>
+      </c>
+      <c r="AA56">
+        <v>443</v>
+      </c>
+      <c r="AB56">
+        <v>5</v>
+      </c>
+      <c r="AC56">
+        <v>65</v>
+      </c>
+      <c r="AD56">
+        <v>140</v>
+      </c>
+      <c r="AE56">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AF56">
+        <v>11</v>
+      </c>
+      <c r="AG56">
+        <v>41</v>
+      </c>
+      <c r="AH56">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="12">
+        <v>45785</v>
+      </c>
+      <c r="D57">
+        <v>14</v>
+      </c>
+      <c r="E57">
+        <v>60</v>
+      </c>
+      <c r="F57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57">
+        <v>155</v>
+      </c>
+      <c r="H57">
+        <v>49.9</v>
+      </c>
+      <c r="I57" t="s">
+        <v>118</v>
+      </c>
+      <c r="J57" t="s">
+        <v>58</v>
+      </c>
+      <c r="K57" s="12">
+        <v>32874</v>
+      </c>
+      <c r="L57" t="s">
+        <v>62</v>
+      </c>
+      <c r="M57" t="s">
+        <v>64</v>
+      </c>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57" t="s">
+        <v>66</v>
+      </c>
+      <c r="S57">
+        <v>127</v>
+      </c>
+      <c r="T57">
+        <v>4.25</v>
+      </c>
+      <c r="U57">
+        <v>6.8</v>
+      </c>
+      <c r="V57">
+        <v>4</v>
+      </c>
+      <c r="W57">
+        <v>2.1</v>
+      </c>
+      <c r="X57">
+        <v>0.5</v>
+      </c>
+      <c r="Y57">
+        <v>0.15</v>
+      </c>
+      <c r="Z57">
+        <v>0.1</v>
+      </c>
+      <c r="AA57">
+        <v>265</v>
+      </c>
+      <c r="AB57">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AC57">
+        <v>72</v>
+      </c>
+      <c r="AD57">
+        <v>139</v>
+      </c>
+      <c r="AE57">
+        <v>4.5</v>
+      </c>
+      <c r="AF57">
+        <v>1</v>
+      </c>
+      <c r="AG57">
+        <v>38</v>
+      </c>
+      <c r="AH57">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="12">
+        <v>45786</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58">
+        <v>18</v>
+      </c>
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58">
+        <v>169.5</v>
+      </c>
+      <c r="H58">
+        <v>58.7</v>
+      </c>
+      <c r="I58" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" t="s">
+        <v>57</v>
+      </c>
+      <c r="K58" s="12">
+        <v>45306</v>
+      </c>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58" t="s">
+        <v>66</v>
+      </c>
+      <c r="S58">
+        <v>126</v>
+      </c>
+      <c r="T58">
+        <v>4.28</v>
+      </c>
+      <c r="U58">
+        <v>6.7</v>
+      </c>
+      <c r="V58">
+        <v>2.8</v>
+      </c>
+      <c r="W58">
+        <v>3</v>
+      </c>
+      <c r="X58">
+        <v>0.4</v>
+      </c>
+      <c r="Y58">
+        <v>0.45</v>
+      </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
+      <c r="AA58">
+        <v>270</v>
+      </c>
+      <c r="AB58">
+        <v>3.4</v>
+      </c>
+      <c r="AC58">
+        <v>46</v>
+      </c>
+      <c r="AD58">
+        <v>138</v>
+      </c>
+      <c r="AE58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AF58">
+        <v>0.5</v>
+      </c>
+      <c r="AG58">
+        <v>39</v>
+      </c>
+      <c r="AH58"/>
+    </row>
+    <row r="59" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="12">
+        <v>45787</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>22</v>
+      </c>
+      <c r="F59" t="s">
+        <v>108</v>
+      </c>
+      <c r="G59">
+        <v>188</v>
+      </c>
+      <c r="H59">
+        <v>82</v>
+      </c>
+      <c r="I59" t="s">
+        <v>117</v>
+      </c>
+      <c r="J59" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" s="12">
+        <v>45444</v>
+      </c>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>71</v>
+      </c>
+      <c r="R59" t="s">
+        <v>67</v>
+      </c>
+      <c r="S59">
+        <v>116</v>
+      </c>
+      <c r="T59">
+        <v>5.28</v>
+      </c>
+      <c r="U59">
+        <v>6.2</v>
+      </c>
+      <c r="V59">
+        <v>2.7</v>
+      </c>
+      <c r="W59">
+        <v>0.4</v>
+      </c>
+      <c r="X59">
+        <v>0.4</v>
+      </c>
+      <c r="Y59">
+        <v>0.13</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
+      <c r="AA59">
+        <v>311</v>
+      </c>
+      <c r="AB59">
+        <v>4.8</v>
+      </c>
+      <c r="AC59">
+        <v>64</v>
+      </c>
+      <c r="AD59">
+        <v>139</v>
+      </c>
+      <c r="AE59">
+        <v>4.3</v>
+      </c>
+      <c r="AF59">
+        <v>0</v>
+      </c>
+      <c r="AG59">
+        <v>40</v>
+      </c>
+      <c r="AH59"/>
+    </row>
+    <row r="60" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="12">
+        <v>45788</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <v>33</v>
+      </c>
+      <c r="F60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60">
+        <v>156</v>
+      </c>
+      <c r="I60" t="s">
+        <v>117</v>
+      </c>
+      <c r="J60" t="s">
+        <v>57</v>
+      </c>
+      <c r="K60" s="12">
+        <v>42908</v>
+      </c>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>72</v>
+      </c>
+      <c r="R60" t="s">
+        <v>66</v>
+      </c>
+      <c r="S60">
+        <v>121</v>
+      </c>
+      <c r="T60">
+        <v>3.59</v>
+      </c>
+      <c r="U60">
+        <v>5.8</v>
+      </c>
+      <c r="V60">
+        <v>4.2</v>
+      </c>
+      <c r="W60">
+        <v>1</v>
+      </c>
+      <c r="X60">
+        <v>0.4</v>
+      </c>
+      <c r="Y60">
+        <v>0.19</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <v>502</v>
+      </c>
+      <c r="AB60">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AC60">
+        <v>52</v>
+      </c>
+      <c r="AD60">
+        <v>143</v>
+      </c>
+      <c r="AE60">
+        <v>4.2</v>
+      </c>
+      <c r="AF60">
+        <v>2.5</v>
+      </c>
+      <c r="AG60">
+        <v>40</v>
+      </c>
+      <c r="AH60">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="12">
+        <v>45789</v>
+      </c>
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>58</v>
+      </c>
+      <c r="F61" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61">
+        <v>169</v>
+      </c>
+      <c r="H61">
+        <v>92</v>
+      </c>
+      <c r="I61" t="s">
+        <v>118</v>
+      </c>
+      <c r="J61" t="s">
+        <v>57</v>
+      </c>
+      <c r="K61" s="12">
+        <v>45091</v>
+      </c>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>73</v>
+      </c>
+      <c r="R61" t="s">
+        <v>66</v>
+      </c>
+      <c r="S61">
+        <v>115</v>
+      </c>
+      <c r="T61">
+        <v>3.82</v>
+      </c>
+      <c r="U61">
+        <v>6.6</v>
+      </c>
+      <c r="V61">
+        <v>3.1</v>
+      </c>
+      <c r="W61">
+        <v>2.5</v>
+      </c>
+      <c r="X61">
+        <v>0.5</v>
+      </c>
+      <c r="Y61">
+        <v>0.51</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <v>286</v>
+      </c>
+      <c r="AB61">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AC61">
+        <v>77</v>
+      </c>
+      <c r="AD61">
+        <v>140</v>
+      </c>
+      <c r="AE61">
+        <v>4.5</v>
+      </c>
+      <c r="AF61">
+        <v>3.5</v>
+      </c>
+      <c r="AG61">
+        <v>37</v>
+      </c>
+      <c r="AH61">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="12">
+        <v>45790</v>
+      </c>
+      <c r="D62">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>17</v>
+      </c>
+      <c r="F62" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62">
+        <v>175</v>
+      </c>
+      <c r="H62">
+        <v>79</v>
+      </c>
+      <c r="I62" t="s">
+        <v>117</v>
+      </c>
+      <c r="J62" t="s">
+        <v>58</v>
+      </c>
+      <c r="K62" s="12">
+        <v>45629</v>
+      </c>
+      <c r="L62" t="s">
+        <v>62</v>
+      </c>
+      <c r="M62" t="s">
+        <v>63</v>
+      </c>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62" t="s">
+        <v>66</v>
+      </c>
+      <c r="S62">
+        <v>127</v>
+      </c>
+      <c r="T62">
+        <v>4.38</v>
+      </c>
+      <c r="U62">
+        <v>7.7</v>
+      </c>
+      <c r="V62">
+        <v>5.3</v>
+      </c>
+      <c r="W62">
+        <v>1.7</v>
+      </c>
+      <c r="X62">
+        <v>0.6</v>
+      </c>
+      <c r="Y62">
+        <v>0.11</v>
+      </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
+      <c r="AA62">
+        <v>341</v>
+      </c>
+      <c r="AB62">
+        <v>5.2</v>
+      </c>
+      <c r="AC62">
+        <v>50</v>
+      </c>
+      <c r="AD62">
+        <v>140</v>
+      </c>
+      <c r="AE62">
+        <v>3.8</v>
+      </c>
+      <c r="AF62">
+        <v>1.56</v>
+      </c>
+      <c r="AG62">
+        <v>37</v>
+      </c>
+      <c r="AH62">
+        <v>732</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>14</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EFF25771-42A9-894F-85CE-5CBBD3C20D30}">
@@ -6616,7 +7385,7 @@
           <x14:formula1>
             <xm:f>data_validation!$AH$2:$AH$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AI4:AW1048576 AJ3:AW3 AI1:AI2 AJ2 AL1:AW2 AK2</xm:sqref>
+          <xm:sqref>AI4:AW1048576 AJ3:AW3 AI1:AI2 AL1:AW2 AJ2:AK2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F5C685B-E7B1-6749-BF4C-93FBC9FD9101}">
           <x14:formula1>
@@ -6631,21 +7400,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView topLeftCell="C9" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.15">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -6653,7 +7422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="22.15">
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -6661,7 +7430,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="22.15">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -6669,24 +7438,24 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="22.15">
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="22.15">
+    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" ht="30">
+    <row r="8" spans="1:2" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="22.15">
+    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -6694,7 +7463,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="22.15">
+    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>84</v>
       </c>
@@ -6702,7 +7471,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="22.15">
+    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>86</v>
       </c>
@@ -6710,7 +7479,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="22.15">
+    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>88</v>
       </c>
@@ -6718,7 +7487,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="22.15">
+    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>90</v>
       </c>
@@ -6726,7 +7495,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="22.15">
+    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>92</v>
       </c>
@@ -6734,7 +7503,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="22.15">
+    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>94</v>
       </c>
@@ -6742,7 +7511,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="22.15">
+    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>96</v>
       </c>
@@ -6750,7 +7519,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="22.15">
+    <row r="17" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>98</v>
       </c>
@@ -6758,7 +7527,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="22.15">
+    <row r="18" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>100</v>
       </c>
@@ -6766,7 +7535,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="22.15">
+    <row r="19" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
@@ -6774,7 +7543,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="22.15">
+    <row r="20" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>104</v>
       </c>
@@ -6782,27 +7551,27 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="1" customFormat="1" ht="30">
+    <row r="22" spans="1:2" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="22.15">
+    <row r="23" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="22.15">
+    <row r="24" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="1" customFormat="1" ht="30">
+    <row r="26" spans="1:2" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="22.15">
+    <row r="27" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>112</v>
       </c>
@@ -6813,20 +7582,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -6972,7 +7741,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>108</v>
       </c>
@@ -7007,7 +7776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>109</v>
       </c>
@@ -7042,7 +7811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
         <v>56</v>
       </c>
@@ -7062,7 +7831,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="P5" t="s">
         <v>74</v>
       </c>

</xml_diff>